<commit_message>
🐛 fix: 初始化指令sleep time順序/insert kd、rsi新增stock_id參數
</commit_message>
<xml_diff>
--- a/app/Form/stock_symbols_01.xlsx
+++ b/app/Form/stock_symbols_01.xlsx
@@ -11,14 +11,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>AAPL</t>
   </si>
   <si>
-    <t>ABNB</t>
-  </si>
-  <si>
     <t>ADBE</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>ARKW</t>
   </si>
   <si>
-    <t>ARKX</t>
-  </si>
-  <si>
     <t>ASML</t>
   </si>
   <si>
@@ -64,7 +58,7 @@
     <t>BIDU</t>
   </si>
   <si>
-    <t>BRK.B</t>
+    <t>BRK-B</t>
   </si>
   <si>
     <t>BYND</t>
@@ -988,16 +982,6 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
🐛 fix: 修改excel data
</commit_message>
<xml_diff>
--- a/app/Form/stock_symbols_01.xlsx
+++ b/app/Form/stock_symbols_01.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>AAPL</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>SNOW</t>
-  </si>
-  <si>
-    <t>SOX</t>
   </si>
   <si>
     <t>SOXX</t>
@@ -993,11 +990,6 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>